<commit_message>
Latest data: Sat Aug 13 09:02:06 UTC 2022
</commit_message>
<xml_diff>
--- a/data_final.xlsx
+++ b/data_final.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,59 +525,152 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Doha</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1008011480150</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Data Entry - Logistics</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>B Holding
+5.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>26d</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1136043&amp;s=58&amp;guid=00000182966fd391874d04224d33b619&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_d048a79d&amp;cb=1660381287641&amp;jobListingId=1008011480150&amp;jrtk=3-0-1gab6vktrihkp801-1gab6vkucimbf800-e68a768aa338085b-</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>We are hiring Administrative Officer with minimum 3 years of experience in Data Entry - Business Analyst - Logistics
+Data Entry Operator Qualifications/Skills:
+Excellent attention to detail.
+Ability to multitask effectively.
+Strong written and verbal communication skills.
+Ability to perform repetitive tasks with a high degree of accuracy.
+Comfortable working independently with minimal supervision.
+Job Types: Full-time, Permanent
+Ability to commute/relocate:
+Doha: Reliably commute or planning to relocate before starting work (Required)
+Education:
+Bachelor's (Preferred)</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>44760</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Qatar</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>1008032650602</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Glassdoor</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>44785</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F3" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>TECHNICAL ASSISTANT</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Qatar Petroleum
 4.0</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>16d</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1136043&amp;s=58&amp;guid=00000182938e7d6788825aff6c13aaae&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_8b5d386f&amp;cb=1660332965712&amp;jobListingId=1008032650602&amp;jrtk=3-0-1ga9osvhrg4dm801-1ga9osvieg2er800-8e4e772d538e8633-</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1136043&amp;s=58&amp;guid=00000182966fd391874d04224d33b619&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_405aabf4&amp;cb=1660381287641&amp;jobListingId=1008032650602&amp;jrtk=3-0-1gab6vktrihkp801-1gab6vkucimbf800-8e4e772d538e8633-</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>Company
 QatarEnergy is an integrated national oil corporation that stands at theforefront of efforts for the long term sustainable
@@ -614,153 +707,8 @@
 Two years Diploma (after high school) in engineering. Good verbal and written command of English is required.</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Company
-QatarEnergy is an integrated national oil corporation that stands at theforefront of efforts for the long term sustainable
-development,utilization and monetization of oil and gas resources in the State ofQatar.In its efforts to become one of the
-best national energy companies inthe world, QatarEnergy's activities and those of its subsidiaries andjoint ventures,
-encompass the entire spectrum of the oil and gas valuechain locally, regionally, and internationally.They include the
-exploration, refining and production, marketing, andsale of oil and gas, liquefied natural gas (LNG), natural gas
-liquids(NGL), gas to liquids (GTL) products, refined products, petrochemicals,fertilizers, steel and aluminum. As an
-integrated corporation,QatarEnergy's activities also include marketing and sale of oil and gasand other various
-products.QatarEnergy's operations and activities are conducted at various onshorelocations, including Doha, Dukhan and
-the Mesaieed and Ras LaffanIndustrial Cities; and at various offshore areas, such as offshore oilfields production stations,
-drilling platforms, Halul oil export island,and the North Field, which is the largest single non-associated gasreservoir in the
-world covering an area of 6,000 square kilometers. Theutilization of this field’s massive reserves has become a
-primarynational goal to continue the development and prosperity of the country.QatarEnergy pays the utmost attention to
-the health and safety of itsemployees, contractors, visitors and the local communities where itoperates. From drilling to
-construction, operations to decommissioning,QatarEnergy's health, safety and environment policy forms an integralpart of
-the corporation’s daily business and long term planning.QatarEnergy is committed to contribute to a better future by
-meetingtoday’s economic needs, while safeguarding our environment and resourcesfor generations to come. Thriving on
-innovation and excellence,QatarEnergy is bound to the highest levels of sustainable human, socio-economic, and
-environmental development in Qatar and beyond.
-Department
-ENGINEERING SERVICES
-Primary purpose of job
-Provide assistance to Lead Document Controller through effective participation in control of engineering documents. Act as
-custodian for archives and also perform data entry, scanning, quality check and uploading documents to the engineering
-information system.
-Provide technical verification of documents received from project execution department for archiving according to QP
-standards and assist in retrieving documents and drawings from the archive and from the technical document management
-system.
-Experience &amp; Skills
-At least 5 years working experience in engineering department with computer systems including document management
-system.
-Education
-Two years Diploma (after high school) in engineering. Good verbal and written command of English is required.</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>44769</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Qatar</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Doha</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1008058062630</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Glassdoor</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>44785</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Data Entry Operator</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Vistas Global
-4.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>5d</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>QAR 78K (Employer est.)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1136043&amp;s=58&amp;guid=00000182938e7d6788825aff6c13aaae&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_4bcabbdb&amp;cb=1660332965712&amp;jobListingId=1008058062630&amp;jrtk=3-0-1ga9osvhrg4dm801-1ga9osvieg2er800-97fc6e9766a3ad08-</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>An esteemed government organization is hiring Data Entry Operator;
-Requirements;
-Should have a minimum of 5 years of experience in the Medical Sector.
-Should at least have a bachelor’s degree. Should have excellent MS Office skills and ERP working knowledge.
-Assist Logistics and SCM Team in the daily transaction, such as delivery, backorder, and item creation.
-Shipped out the outbound transaction through ERP System.
-Assess and resolve issues related to excess quantity, duplicate orders (item code and description), and discontinued items.
-Performing logical transaction data in Oracle as per SCM team request.</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>An esteemed government organization is hiring Data Entry Operator;
-Requirements;
-Should have a minimum of 5 years of experience in the Medical Sector.
-Should at least have a bachelor’s degree. Should have excellent MS Office skills and ERP working knowledge.
-Assist Logistics and SCM Team in the daily transaction, such as delivery, backorder, and item creation.
-Shipped out the outbound transaction through ERP System.
-Assess and resolve issues related to excess quantity, duplicate orders (item code and description), and discontinued items.
-Performing logical transaction data in Oracle as per SCM team request.
-Update sub-inventory, quantity, and lot expiry of the item. Submit a request for a back-ordered item.
-Update the master list to avoid item duplication. Responsible for tracking orders and order creation.
-Escalate order creation issue and report to Clinical Supply Chain Management Supervisor.
-Assisting Data Entry Operator in resolving the ERP transaction issue. Assisting with SCM team for outbound reconciliation.
-Responsible for all outbound transactions performed in Oracle without any pending.
-Coordinate activities with the Logistics Team to ensure timely approval of Requisitions.
-Shared expired item details and P.O details daily as per Storekeepers’ request. Entering data into a database.
-Participate in yearly stock counting in Health Center and Central Warehouse and report any discrepancy to the SCM team.
-Follow office workflow procedures to ensure maximum efficiency
-Support meeting and conferencing needs. Maintain files and records with effective filing systems
-Job Type: Full-time
-Salary: QAR6,500.00 per month
-Education:
-Bachelor's (Preferred)
-Experience:
-Medical Sector: 5 years (Preferred)
-Arabic (Preferred)</t>
-        </is>
-      </c>
       <c r="P3" s="2" t="n">
-        <v>44780</v>
+        <v>44770</v>
       </c>
     </row>
     <row r="4">
@@ -779,7 +727,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1007567176042</t>
+          <t>1008049422541</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -788,76 +736,380 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Data Entry Operator (Medical Sector)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>BPO PLUS
+3.1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>10d</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>QAR 48K - QAR 72K (Employer est.)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Full-time, Contract</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1136043&amp;s=58&amp;guid=00000182966fd391874d04224d33b619&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_4119e6fa&amp;cb=1660381287641&amp;jobListingId=1008049422541&amp;jrtk=3-0-1gab6vktrihkp801-1gab6vkucimbf800-4f0bf10e817d77cf-</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Position Title: Data Entry Operator (Medical Sector)
+Qualification:
+Bachelor’s Degree in business administration or its equivalent
+Experience &amp; Knowledge Requirement:
+Minimum 5 years of experience Data Entry in the Medical Sector, computer-savvy with a working knowledge of logistics software (ERP).
+Skills Requirements:
+Microsoft office skills.
+Good communication skills
+Customer Oriented
+Time Management
+Major Responsibilities:
+Assist Logistics and SCM Team in the daily transaction, such as delivery, backorder and item creation.
+Shipped out the outbound transaction through ERP System.
+Assess and resolve issues related to excess quantity, duplicate orders (item code and description), and discontinued items.
+Performing logical transaction data in Oracle as per SCM team request.
+Update sub-inventory, quantity, and lot expiry of the item.
+Submit a request for a backordered item.
+Update the master list to avoid item duplication.
+Responsible for tracking orders and order creation.
+Escalate order creation issue and report to Clinical Supply Chain Management Supervisor.
+Assisting Data Entry Operator in resolving the ERP transaction issue.
+Assisting with SCM team for outbound reconciliation.
+Responsible for all outbound transactions performing in Oracle without any pending.
+Coordinate activities with the Logistics Team to ensure timely approval of Requisitions.
+Shared expired item details and P.O details daily as per Storekeepers’ request.
+Participate in yearly stock counting in Health Center and Central Warehouse and report any discrepancy to the SCM team.
+Follow office workflow procedures to ensure maximum efficiency
+Support meeting and conferencing needs.
+Maintain files and records with effective filing systems
+Job Types: Full-time, Contract
+Contract length: 36 months
+Salary: QAR4,000.00 - QAR6,000.00 per month
+Education:
+Bachelor's (Required)
+Experience:
+Data Entry in the Medical Sector: 5 years (Required)
+License/Certification:
+Qatar ID (Required)</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Birmingham, England</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1008066425644</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>University Hospitals Birmingham
+3.6</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2d</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>£27K - £33K (Employer est.)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1136043&amp;s=58&amp;guid=0000018296703b3091b079ec3d7ac7f7&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_e1733370&amp;cb=1660381314235&amp;jobListingId=1008066425644&amp;jrtk=3-0-1gab70eqkgrgm801-1gab70er7ghrk800-de0732b2f020cc33-</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>At University Hospitals Birmingham our teams are committed to building healthier lives – this includes our colleagues as well as patients.
+To ensure we are continually developing our services to all departments, our Health Informatics team support the provision of data services to all areas of the Trust. With growing demands on the team, a new opportunity for a Data Analyst has been created to support the provision of data services across the Trust.
+You as the successful candidate, will work with clinical, operational and corporate data to support a variety of project-based and ad-hoc work. You will use your previous analytical experience gained in either academic or professional settings.
+In addition, you will have a foundation in technical scripting/programming. Experience of; SQL, Power BI, SQL Server (SSMS, SSIS, SSRS), R, Python is desirable but not essential.
+To be effective in this role you will have keen attention to detail, and be proactive in improving data quality and increasing automation. You will be able to demonstrate your numeracy and analytical skills at assessment and interview.
+In return you can expect to join like minded people who deliver unequivocal excellence in all aspects of their role, who are encouraged by their peers to deliver on their individual ability and creativity and who continue to drive the department’s innovations. You will compliment this team, with your ability to think through complex problems, always driving continuous improvement and developing best practices in Informatics.
+In return you can expect to join Birmingham and Solihull’s largest employer where you will have a direct impact on how we care for our patients. You can expect a starting salary of £27,055 rising to £32,934, along with 27 days leave plus bank holidays and enrolment onto the renowned NHS Pension Scheme.
+Interested applicants are invited to get in touch with Jerry Orme, Clinical Intelligence Analyst, at jerry.orme at uhb.nhs.uk for an informal chat.
+Job Types: Full-time, Permanent
+Salary: £27,055.00-£32,934.00 per year
+Benefits:
+On-site parking
+Work from home
+Schedule:
+8 hour shift
+Day shift
+Monday to Friday
+Application deadline: 29/08/2022
+Reference ID: HJ-JR-DA</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>44784</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sunderland, North East England, England</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1008062303595</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>South Tyneside and Sunderland NHS Foundation Trust
+3.3</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>3d</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>£26K - £32K (Employer est.)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1136043&amp;s=58&amp;guid=0000018296703b3091b079ec3d7ac7f7&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_78771bd1&amp;cb=1660381314235&amp;jobListingId=1008062303595&amp;jrtk=3-0-1gab70eqkgrgm801-1gab70er7ghrk800-4d5c7ad9ab5f54e1-</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Please switch to a desktop device before starting your application.
+An exciting opportunity has arisen within the Information Services team for a Data Analyst to support the organisation with the development of reporting of high quality and timely information both internally and externally to support operational needs. We are looking for someone who has experience of data extraction, analysis and visualisation techniques, with strong customer service and communication skills.
+Please note there are 2 posts available;
+1x full time permanent and 1x full time fixed term for 12 months. Secondment applications are welcomed.
+Interviews are scheduled for 7th September 2022.</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>44783</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Newry, Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1008067974056</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Glassdoor</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Re-Gen Waste
+3.3</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1d</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>£27K - £34K (Glassdoor est.)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1136043&amp;s=58&amp;guid=0000018296703b3091b079ec3d7ac7f7&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;ea=1&amp;cs=1_4bd3d558&amp;cb=1660381314235&amp;jobListingId=1008067974056&amp;jrtk=3-0-1gab70eqkgrgm801-1gab70er7ghrk800-e9822886b14d8db6-</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Job Overview:
+Due to increased workload, we are currently recruiting for the role of Data Analyst reporting to the IT Manager whilst working with a number of departments across the business based within our Head Office in Newry. As a Data Analyst you will manage the data, present reports to the business and liaise with department heads on establishing best solutions and improvements that can be implemented.
+This is an excellent opportunity to join an exciting and expanding Company where you will have wide exposure to various data platforms and support to also develop your skills.
+Key Duties:
+· Capture, Analyse and Present Business Data to assist with strategic decisions
+· Design Reports and Dashboards for Business Units
+· Automate Data Capture for Business Departments
+· Apply AI and ML to Datasets
+· Identify Patterns and insights from Company Data
+· Communicate key information to Stakeholders
+· Ability to work in a fast-paced environment
+· Any other duties deemed necessary by management
+Essential Criteria:
+· Hold or be working towards Third level qualification in Computer Science, Maths, Science, Business or Similar field to at least a 2.1
+· Programming Experience in one or more of R/SAS/Python/SQL
+· Data Presentation Skills in Tableau/Power BI or Similar
+· Ability to work toward tight schedules and deadlines and problem solving
+· Excellent communication skills both verbal and written
+· Excellent organisational and analytical skills
+· Full Driving Licence and access to own transport
+Desirable Criteria:
+· At least 6 months’ relevant work or research experience
+Duration: Full Time Permanent
+Location: Newry
+Remuneration: Attractive
+Hours of work: 8am to 5pm
+Benefits: Free Life Assurance, Company Pension Scheme, Healthcare Plan, Paid holidays, Employee Perks Card, Free On-site car parking, Canteen Facilities, Career Development Opportunities, possible option for hybrid working etc.
+Re-Gen is an equal opportunities employer who employs a workforce with members from all sections of the community and is committed to appointing candidates purely based on merit
+Job Type: Full-time
+Schedule:
+Day shift
+Monday to Friday
+Work authorisation:
+United Kingdom (required)
+Application deadline: 17/08/2022</t>
+        </is>
+      </c>
+      <c r="P7" s="2" t="n">
         <v>44785</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Data Scientist - Advanced Analytics</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>McKinsey &amp; Company
-4.4</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>4.4</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>30d+</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1136043&amp;s=58&amp;guid=00000182938e7d6788825aff6c13aaae&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;cs=1_f6ebb6d9&amp;cb=1660332965712&amp;jobListingId=1007567176042&amp;jrtk=3-0-1ga9osvhrg4dm801-1ga9osvieg2er800-777b91555ee9b1eb-</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Who You'll Work With
-You will be based in our Riyadh, Saudi Arabia or Doha, Qatar office as part of our Advanced Analytics team, partnering with consultants, clients, and other colleagues.
-Our Advanced Analytics teams bring the latest analytical techniques plus a deep understanding of industry dynamics and corporate functions to help clients create the most value from data.
-What You'll Do
-You will use data creatively to solve business challenges, often uncovering new and transformative opportunities along the way.
-In this role, you will focus on the development of advanced analytics models to optimize underlying business problems. You will apply state-of-the-art advanced analytics, quantitative tools and modeling techniques to interpret, make inferences and offer recommendations based on insights from the data. You will shape the future of what data-driven organizations look like, drive processes for extracting and using that data in creative ways and create new lines of thinking within an infinite number of clients and situations.</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Who You'll Work With
-You will be based in our Riyadh, Saudi Arabia or Doha, Qatar office as part of our Advanced Analytics team, partnering with consultants, clients, and other colleagues.
-Our Advanced Analytics teams bring the latest analytical techniques plus a deep understanding of industry dynamics and corporate functions to help clients create the most value from data.
-What You'll Do
-You will use data creatively to solve business challenges, often uncovering new and transformative opportunities along the way.
-In this role, you will focus on the development of advanced analytics models to optimize underlying business problems. You will apply state-of-the-art advanced analytics, quantitative tools and modeling techniques to interpret, make inferences and offer recommendations based on insights from the data. You will shape the future of what data-driven organizations look like, drive processes for extracting and using that data in creative ways and create new lines of thinking within an infinite number of clients and situations.
-You will create valuable, transformative business strategies through the measurement, manipulation, reporting and dissemination of broad sets of data. You will apply and advise on state-of-the-art advanced analytic and quantitative tools and modeling techniques in order to derive business insights, solve complex business problems and improve decisions. You will review, support and advise on the day-to-day analytics requirements of clients’ key operational processes while continually improving the impact of these processes.
-Qualifications
-Undergraduate degree in mathematics, statistics, physics, engineering; master's degree is a plus
-3+ years of professional experience in programming; experience applied to business problems is a plus
-Experience in programming (focus on machine learning) in Python and/or R; knowledge in SPSS, SAS, Ruby, Hadoop is a plus
-Experience in data treatment/data mining: SQL, AWK, Access, Spark, Excel
-Demonstrated aptitude for analytics; statistical knowledge is a plus
-Proven record of leadership in a work setting and/or through extracurricular activities
-Ability to work collaboratively in a team environment and effectively with people at all levels in an organization
-Ability to communicate complex ideas effectively, both verbally and in writing, in English; fluency in local office language(s) is a plus</t>
-        </is>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>44755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>